<commit_message>
Strings, Logical- And, or, If
</commit_message>
<xml_diff>
--- a/Excel/Data files/Lecture_1.xlsx
+++ b/Excel/Data files/Lecture_1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E196161-7545-49D4-830C-6C8CC8AF3E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCB26AF-F2D2-4E55-9F57-F93F03C71404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="53">
   <si>
     <t>SUM</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>MOD</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -534,6 +543,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -588,14 +605,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1456,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1480,10 +1489,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="52"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1491,24 +1500,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1517,13 +1526,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -1546,11 +1555,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -1567,17 +1576,13 @@
       <c r="O5" s="25">
         <v>81</v>
       </c>
-      <c r="P5">
-        <f>SUM(M5:O5)</f>
-        <v>259</v>
-      </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -1590,17 +1595,13 @@
       <c r="O6" s="25">
         <v>75</v>
       </c>
-      <c r="P6">
-        <f t="shared" ref="P6:P9" si="0">SUM(M6:O6)</f>
-        <v>193</v>
-      </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -1613,17 +1614,13 @@
       <c r="O7" s="25">
         <v>90</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -1636,17 +1633,13 @@
       <c r="O8" s="25">
         <v>85</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>283</v>
-      </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -1659,40 +1652,24 @@
       <c r="O9" s="25">
         <v>55</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
-      <c r="L10" s="54" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
+      <c r="L10" s="35" t="s">
         <v>44</v>
-      </c>
-      <c r="M10">
-        <f>SUM(M5:M9)</f>
-        <v>389</v>
-      </c>
-      <c r="N10">
-        <f t="shared" ref="N10:O10" si="1">SUM(N5:N9)</f>
-        <v>375</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="1"/>
-        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -1703,84 +1680,84 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="53"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
     </row>
     <row r="17" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="C4:G11"/>
     <mergeCell ref="C14:G21"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1791,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:G11"/>
+    <sheetView showGridLines="0" zoomScale="76" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1815,10 +1792,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="52"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1826,24 +1803,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1852,13 +1829,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -1878,11 +1855,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -1901,11 +1878,11 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -1920,11 +1897,11 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -1939,11 +1916,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -1958,11 +1935,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -1977,34 +1954,34 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="L10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="55">
+      <c r="M10" s="36">
         <f>MIN(M5:M9)</f>
         <v>45</v>
       </c>
-      <c r="N10" s="55">
+      <c r="N10" s="36">
         <f t="shared" ref="N10:O10" si="0">MIN(N5:N9)</f>
         <v>53</v>
       </c>
-      <c r="O10" s="55">
+      <c r="O10" s="36">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -2015,64 +1992,64 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2097,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2121,10 +2098,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="52"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2132,24 +2109,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2158,13 +2135,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2184,11 +2161,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -2207,11 +2184,11 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -2226,11 +2203,11 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -2245,11 +2222,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -2264,11 +2241,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -2283,34 +2260,34 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="L10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="55">
+      <c r="M10" s="36">
         <f>MAX(M5:M9)</f>
         <v>99</v>
       </c>
-      <c r="N10" s="55">
-        <f>MAX(N5:N9)</f>
+      <c r="N10" s="36">
+        <f t="shared" ref="N10:O10" si="0">MAX(N5:N9)</f>
         <v>99</v>
       </c>
-      <c r="O10" s="55">
-        <f t="shared" ref="N10:O10" si="0">MAX(O5:O9)</f>
+      <c r="O10" s="36">
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
       <c r="N11" t="s">
         <v>45</v>
       </c>
@@ -2327,64 +2304,64 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2410,7 +2387,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="83" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:P9"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2433,10 +2410,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="52"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2444,24 +2421,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2470,13 +2447,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2502,11 +2479,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -2523,21 +2500,21 @@
       <c r="O5" s="25">
         <v>81</v>
       </c>
-      <c r="P5" s="55">
+      <c r="P5" s="36">
         <f>AVERAGE(M5:O5)</f>
         <v>86.333333333333329</v>
       </c>
-      <c r="Q5" s="55">
+      <c r="Q5" s="36">
         <f>_xlfn.RANK.AVG(P5,$P$5:$P$9,0)</f>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -2550,21 +2527,21 @@
       <c r="O6" s="25">
         <v>75</v>
       </c>
-      <c r="P6" s="55">
+      <c r="P6" s="36">
         <f t="shared" ref="P6:P9" si="0">AVERAGE(M6:O6)</f>
         <v>64.333333333333329</v>
       </c>
-      <c r="Q6" s="55">
+      <c r="Q6" s="36">
         <f t="shared" ref="Q6:Q9" si="1">_xlfn.RANK.AVG(P6,$P$5:$P$9,0)</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -2577,21 +2554,21 @@
       <c r="O7" s="25">
         <v>90</v>
       </c>
-      <c r="P7" s="55">
+      <c r="P7" s="36">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="Q7" s="55">
+      <c r="Q7" s="36">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -2604,21 +2581,21 @@
       <c r="O8" s="25">
         <v>85</v>
       </c>
-      <c r="P8" s="55">
+      <c r="P8" s="36">
         <f t="shared" si="0"/>
         <v>94.333333333333329</v>
       </c>
-      <c r="Q8" s="55">
+      <c r="Q8" s="36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -2631,29 +2608,29 @@
       <c r="O9" s="25">
         <v>55</v>
       </c>
-      <c r="P9" s="55">
+      <c r="P9" s="36">
         <f t="shared" si="0"/>
         <v>53.333333333333336</v>
       </c>
-      <c r="Q9" s="55">
+      <c r="Q9" s="36">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -2664,64 +2641,64 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2747,7 +2724,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2783,24 +2760,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2809,13 +2786,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2838,11 +2815,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -2865,11 +2842,11 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -2888,11 +2865,11 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -2911,11 +2888,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -2934,11 +2911,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -2957,11 +2934,11 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -2969,11 +2946,11 @@
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
       <c r="L11" s="27" t="s">
         <v>28</v>
       </c>
@@ -3010,43 +2987,43 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="L14" s="22"/>
       <c r="M14" s="23"/>
       <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
       <c r="L15" s="21"/>
       <c r="M15" s="23"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
       <c r="L16" s="21"/>
       <c r="M16" s="23"/>
     </row>
     <row r="17" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
       <c r="L17" s="21"/>
       <c r="M17" s="23">
         <f>M5*M11+N5*N11+O5*O11</f>
@@ -3057,11 +3034,11 @@
       </c>
     </row>
     <row r="18" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
       <c r="L18" s="21"/>
       <c r="M18" s="23"/>
       <c r="N18" t="s">
@@ -3069,20 +3046,20 @@
       </c>
     </row>
     <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
     </row>
     <row r="20" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -3091,11 +3068,11 @@
       <c r="Q20" s="21"/>
     </row>
     <row r="21" spans="3:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3119,8 +3096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:M18"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3154,24 +3131,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3180,13 +3157,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -3207,11 +3184,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -3231,11 +3208,11 @@
       <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -3251,11 +3228,11 @@
       <c r="P6" s="26"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -3271,11 +3248,11 @@
       <c r="P7" s="26"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -3291,11 +3268,11 @@
       <c r="P8" s="26"/>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -3311,11 +3288,11 @@
       <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -3324,11 +3301,11 @@
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
       <c r="L11" s="31" t="s">
         <v>37</v>
       </c>
@@ -3360,189 +3337,173 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="L14" s="25" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="25">
         <f ca="1">RAND()</f>
-        <v>0.39179767679898891</v>
+        <v>0.4837099809054286</v>
       </c>
       <c r="N14" s="26">
         <f ca="1">RAND()*10</f>
-        <v>4.7880850903969652</v>
+        <v>1.6781308214022495</v>
       </c>
       <c r="O14" s="26">
         <f ca="1">RAND()*99</f>
-        <v>40.602067827870556</v>
+        <v>83.889817383946763</v>
       </c>
       <c r="P14" s="26">
-        <f ca="1">INT(RAND()*20)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
       <c r="L15" s="25" t="s">
         <v>31</v>
       </c>
       <c r="M15" s="25">
         <f t="shared" ref="M15:M18" ca="1" si="0">RAND()</f>
-        <v>0.71965135468382491</v>
+        <v>0.63392973555310439</v>
       </c>
       <c r="N15" s="26">
         <f t="shared" ref="N15:N18" ca="1" si="1">RAND()*10</f>
-        <v>8.9020014507213272</v>
+        <v>4.5404036720694005</v>
       </c>
       <c r="O15" s="26">
         <f t="shared" ref="O15:O18" ca="1" si="2">RAND()*99</f>
-        <v>56.436969233560909</v>
-      </c>
-      <c r="P15" s="26">
-        <f t="shared" ref="P15:P22" ca="1" si="3">INT(RAND()*20)</f>
-        <v>11</v>
+        <v>14.383007218579877</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
       <c r="L16" s="25" t="s">
         <v>32</v>
       </c>
       <c r="M16" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67150279467617635</v>
+        <v>5.5591008335340031E-2</v>
       </c>
       <c r="N16" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4604784344691542</v>
+        <v>1.4768955398234906</v>
       </c>
       <c r="O16" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>53.519638576045139</v>
-      </c>
-      <c r="P16" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+        <v>69.902242056228005</v>
+      </c>
+      <c r="P16" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
       <c r="L17" s="25" t="s">
         <v>33</v>
       </c>
       <c r="M17" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61123066356751754</v>
+        <v>0.77662376364453611</v>
       </c>
       <c r="N17" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2527811712379053</v>
+        <v>4.4234228277888334</v>
       </c>
       <c r="O17" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76273354713847574</v>
+        <v>56.342323106026839</v>
       </c>
       <c r="P17" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
       <c r="L18" s="25" t="s">
         <v>34</v>
       </c>
       <c r="M18" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1795626763216158E-2</v>
+        <v>0.79484219417391622</v>
       </c>
       <c r="N18" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0661480338569591</v>
+        <v>2.265552251904829</v>
       </c>
       <c r="O18" s="26">
         <f t="shared" ca="1" si="2"/>
-        <v>67.607998893363487</v>
-      </c>
-      <c r="P18" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+        <v>40.916827583418254</v>
+      </c>
+      <c r="P18" s="26"/>
+      <c r="Q18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
-      <c r="P19" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
       <c r="N20" s="26"/>
       <c r="O20" s="26"/>
-      <c r="P20" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="3:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" spans="3:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
-      <c r="P21" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="P22" s="26">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3567,7 +3528,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="M13" sqref="M13:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3601,24 +3562,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3627,13 +3588,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -3653,11 +3614,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -3676,11 +3637,11 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="25" t="s">
         <v>31</v>
       </c>
@@ -3695,11 +3656,11 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="25" t="s">
         <v>32</v>
       </c>
@@ -3714,11 +3675,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
@@ -3733,11 +3694,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="25" t="s">
         <v>34</v>
       </c>
@@ -3752,34 +3713,34 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="L10" s="33" t="s">
         <v>39</v>
       </c>
       <c r="M10" s="25">
         <f ca="1">RANDBETWEEN(35,70)</f>
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N10" s="25">
         <f t="shared" ref="N10:O10" ca="1" si="0">RANDBETWEEN(35,70)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="O10" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
     </row>
@@ -3796,76 +3757,76 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
       <c r="N16" s="26"/>
       <c r="O16" s="26"/>
     </row>
     <row r="17" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
     </row>
     <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
     </row>
     <row r="19" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
     </row>
     <row r="20" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3890,7 +3851,7 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3924,24 +3885,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>

</xml_diff>